<commit_message>
Actualizar ligas y agregar Liga Argentina actualizada
</commit_message>
<xml_diff>
--- a/Ligas/Liga_MLS_2025.xlsx
+++ b/Ligas/Liga_MLS_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S337"/>
+  <dimension ref="A1:S351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23158,6 +23158,1000 @@
         </is>
       </c>
     </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>New York Red Bulls</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Inter Miami</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>1</v>
+      </c>
+      <c r="E338" t="n">
+        <v>5</v>
+      </c>
+      <c r="F338" t="n">
+        <v>1326555</v>
+      </c>
+      <c r="G338" t="n">
+        <v>2</v>
+      </c>
+      <c r="H338" t="n">
+        <v>4</v>
+      </c>
+      <c r="I338" t="n">
+        <v>2</v>
+      </c>
+      <c r="J338" t="n">
+        <v>3</v>
+      </c>
+      <c r="K338" t="n">
+        <v>0</v>
+      </c>
+      <c r="L338" t="n">
+        <v>0</v>
+      </c>
+      <c r="M338" t="n">
+        <v>0</v>
+      </c>
+      <c r="N338" t="n">
+        <v>0</v>
+      </c>
+      <c r="O338" t="n">
+        <v>1</v>
+      </c>
+      <c r="P338" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q338" t="inlineStr">
+        <is>
+          <t>37%</t>
+        </is>
+      </c>
+      <c r="R338" t="inlineStr">
+        <is>
+          <t>63%</t>
+        </is>
+      </c>
+      <c r="S338" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Atlanta United FC</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>2</v>
+      </c>
+      <c r="E339" t="n">
+        <v>3</v>
+      </c>
+      <c r="F339" t="n">
+        <v>1326551</v>
+      </c>
+      <c r="G339" t="n">
+        <v>7</v>
+      </c>
+      <c r="H339" t="n">
+        <v>2</v>
+      </c>
+      <c r="I339" t="n">
+        <v>1</v>
+      </c>
+      <c r="J339" t="n">
+        <v>1</v>
+      </c>
+      <c r="K339" t="n">
+        <v>0</v>
+      </c>
+      <c r="L339" t="n">
+        <v>0</v>
+      </c>
+      <c r="M339" t="n">
+        <v>0</v>
+      </c>
+      <c r="N339" t="n">
+        <v>0</v>
+      </c>
+      <c r="O339" t="n">
+        <v>2</v>
+      </c>
+      <c r="P339" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q339" t="inlineStr">
+        <is>
+          <t>54%</t>
+        </is>
+      </c>
+      <c r="R339" t="inlineStr">
+        <is>
+          <t>46%</t>
+        </is>
+      </c>
+      <c r="S339" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>1</v>
+      </c>
+      <c r="E340" t="n">
+        <v>2</v>
+      </c>
+      <c r="F340" t="n">
+        <v>1326554</v>
+      </c>
+      <c r="G340" t="n">
+        <v>9</v>
+      </c>
+      <c r="H340" t="n">
+        <v>6</v>
+      </c>
+      <c r="I340" t="n">
+        <v>2</v>
+      </c>
+      <c r="J340" t="n">
+        <v>2</v>
+      </c>
+      <c r="K340" t="n">
+        <v>0</v>
+      </c>
+      <c r="L340" t="n">
+        <v>0</v>
+      </c>
+      <c r="M340" t="n">
+        <v>0</v>
+      </c>
+      <c r="N340" t="n">
+        <v>0</v>
+      </c>
+      <c r="O340" t="n">
+        <v>1</v>
+      </c>
+      <c r="P340" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q340" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="R340" t="inlineStr">
+        <is>
+          <t>38%</t>
+        </is>
+      </c>
+      <c r="S340" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2025-07-19</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>CF Montreal</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>0</v>
+      </c>
+      <c r="E341" t="n">
+        <v>2</v>
+      </c>
+      <c r="F341" t="n">
+        <v>1326553</v>
+      </c>
+      <c r="G341" t="n">
+        <v>5</v>
+      </c>
+      <c r="H341" t="n">
+        <v>3</v>
+      </c>
+      <c r="I341" t="n">
+        <v>4</v>
+      </c>
+      <c r="J341" t="n">
+        <v>3</v>
+      </c>
+      <c r="K341" t="n">
+        <v>0</v>
+      </c>
+      <c r="L341" t="n">
+        <v>0</v>
+      </c>
+      <c r="M341" t="n">
+        <v>0</v>
+      </c>
+      <c r="N341" t="n">
+        <v>0</v>
+      </c>
+      <c r="O341" t="n">
+        <v>0</v>
+      </c>
+      <c r="P341" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q341" t="inlineStr">
+        <is>
+          <t>51%</t>
+        </is>
+      </c>
+      <c r="R341" t="inlineStr">
+        <is>
+          <t>49%</t>
+        </is>
+      </c>
+      <c r="S341" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Columbus Crew</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>DC United</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>2</v>
+      </c>
+      <c r="E342" t="n">
+        <v>1</v>
+      </c>
+      <c r="F342" t="n">
+        <v>1326552</v>
+      </c>
+      <c r="G342" t="n">
+        <v>7</v>
+      </c>
+      <c r="H342" t="n">
+        <v>0</v>
+      </c>
+      <c r="I342" t="n">
+        <v>1</v>
+      </c>
+      <c r="J342" t="n">
+        <v>2</v>
+      </c>
+      <c r="K342" t="n">
+        <v>0</v>
+      </c>
+      <c r="L342" t="n">
+        <v>1</v>
+      </c>
+      <c r="M342" t="n">
+        <v>0</v>
+      </c>
+      <c r="N342" t="n">
+        <v>0</v>
+      </c>
+      <c r="O342" t="n">
+        <v>2</v>
+      </c>
+      <c r="P342" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q342" t="inlineStr">
+        <is>
+          <t>64%</t>
+        </is>
+      </c>
+      <c r="R342" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
+      <c r="S342" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Seattle Sounders</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>San Jose Earthquakes</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>3</v>
+      </c>
+      <c r="E343" t="n">
+        <v>2</v>
+      </c>
+      <c r="F343" t="n">
+        <v>1326560</v>
+      </c>
+      <c r="G343" t="n">
+        <v>5</v>
+      </c>
+      <c r="H343" t="n">
+        <v>2</v>
+      </c>
+      <c r="I343" t="n">
+        <v>1</v>
+      </c>
+      <c r="J343" t="n">
+        <v>3</v>
+      </c>
+      <c r="K343" t="n">
+        <v>0</v>
+      </c>
+      <c r="L343" t="n">
+        <v>0</v>
+      </c>
+      <c r="M343" t="n">
+        <v>0</v>
+      </c>
+      <c r="N343" t="n">
+        <v>0</v>
+      </c>
+      <c r="O343" t="n">
+        <v>3</v>
+      </c>
+      <c r="P343" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q343" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="R343" t="inlineStr">
+        <is>
+          <t>47%</t>
+        </is>
+      </c>
+      <c r="S343" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>FC Dallas</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>St. Louis City</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>3</v>
+      </c>
+      <c r="E344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F344" t="n">
+        <v>1326556</v>
+      </c>
+      <c r="G344" t="n">
+        <v>2</v>
+      </c>
+      <c r="H344" t="n">
+        <v>4</v>
+      </c>
+      <c r="I344" t="n">
+        <v>2</v>
+      </c>
+      <c r="J344" t="n">
+        <v>0</v>
+      </c>
+      <c r="K344" t="n">
+        <v>0</v>
+      </c>
+      <c r="L344" t="n">
+        <v>0</v>
+      </c>
+      <c r="M344" t="n">
+        <v>0</v>
+      </c>
+      <c r="N344" t="n">
+        <v>0</v>
+      </c>
+      <c r="O344" t="n">
+        <v>3</v>
+      </c>
+      <c r="P344" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q344" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="R344" t="inlineStr">
+        <is>
+          <t>66%</t>
+        </is>
+      </c>
+      <c r="S344" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Houston Dynamo</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Philadelphia Union</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>1</v>
+      </c>
+      <c r="E345" t="n">
+        <v>1</v>
+      </c>
+      <c r="F345" t="n">
+        <v>1326557</v>
+      </c>
+      <c r="G345" t="n">
+        <v>2</v>
+      </c>
+      <c r="H345" t="n">
+        <v>4</v>
+      </c>
+      <c r="I345" t="n">
+        <v>3</v>
+      </c>
+      <c r="J345" t="n">
+        <v>4</v>
+      </c>
+      <c r="K345" t="n">
+        <v>0</v>
+      </c>
+      <c r="L345" t="n">
+        <v>1</v>
+      </c>
+      <c r="M345" t="n">
+        <v>0</v>
+      </c>
+      <c r="N345" t="n">
+        <v>0</v>
+      </c>
+      <c r="O345" t="n">
+        <v>1</v>
+      </c>
+      <c r="P345" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q345" t="inlineStr">
+        <is>
+          <t>61%</t>
+        </is>
+      </c>
+      <c r="R345" t="inlineStr">
+        <is>
+          <t>39%</t>
+        </is>
+      </c>
+      <c r="S345" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Sporting Kansas City</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>1</v>
+      </c>
+      <c r="E346" t="n">
+        <v>1</v>
+      </c>
+      <c r="F346" t="n">
+        <v>1326558</v>
+      </c>
+      <c r="G346" t="n">
+        <v>7</v>
+      </c>
+      <c r="H346" t="n">
+        <v>4</v>
+      </c>
+      <c r="I346" t="n">
+        <v>2</v>
+      </c>
+      <c r="J346" t="n">
+        <v>0</v>
+      </c>
+      <c r="K346" t="n">
+        <v>0</v>
+      </c>
+      <c r="L346" t="n">
+        <v>0</v>
+      </c>
+      <c r="M346" t="n">
+        <v>0</v>
+      </c>
+      <c r="N346" t="n">
+        <v>0</v>
+      </c>
+      <c r="O346" t="n">
+        <v>1</v>
+      </c>
+      <c r="P346" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q346" t="inlineStr">
+        <is>
+          <t>39%</t>
+        </is>
+      </c>
+      <c r="R346" t="inlineStr">
+        <is>
+          <t>61%</t>
+        </is>
+      </c>
+      <c r="S346" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Nashville SC</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>1</v>
+      </c>
+      <c r="E347" t="n">
+        <v>0</v>
+      </c>
+      <c r="F347" t="n">
+        <v>1326559</v>
+      </c>
+      <c r="G347" t="n">
+        <v>6</v>
+      </c>
+      <c r="H347" t="n">
+        <v>2</v>
+      </c>
+      <c r="I347" t="n">
+        <v>3</v>
+      </c>
+      <c r="J347" t="n">
+        <v>2</v>
+      </c>
+      <c r="K347" t="n">
+        <v>0</v>
+      </c>
+      <c r="L347" t="n">
+        <v>0</v>
+      </c>
+      <c r="M347" t="n">
+        <v>0</v>
+      </c>
+      <c r="N347" t="n">
+        <v>0</v>
+      </c>
+      <c r="O347" t="n">
+        <v>1</v>
+      </c>
+      <c r="P347" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q347" t="inlineStr">
+        <is>
+          <t>52%</t>
+        </is>
+      </c>
+      <c r="R347" t="inlineStr">
+        <is>
+          <t>48%</t>
+        </is>
+      </c>
+      <c r="S347" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Real Salt Lake</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>FC Cincinnati</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>0</v>
+      </c>
+      <c r="E348" t="n">
+        <v>1</v>
+      </c>
+      <c r="F348" t="n">
+        <v>1326561</v>
+      </c>
+      <c r="G348" t="n">
+        <v>3</v>
+      </c>
+      <c r="H348" t="n">
+        <v>5</v>
+      </c>
+      <c r="I348" t="n">
+        <v>2</v>
+      </c>
+      <c r="J348" t="n">
+        <v>4</v>
+      </c>
+      <c r="K348" t="n">
+        <v>0</v>
+      </c>
+      <c r="L348" t="n">
+        <v>0</v>
+      </c>
+      <c r="M348" t="n">
+        <v>0</v>
+      </c>
+      <c r="N348" t="n">
+        <v>0</v>
+      </c>
+      <c r="O348" t="n">
+        <v>0</v>
+      </c>
+      <c r="P348" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q348" t="inlineStr">
+        <is>
+          <t>57%</t>
+        </is>
+      </c>
+      <c r="R348" t="inlineStr">
+        <is>
+          <t>43%</t>
+        </is>
+      </c>
+      <c r="S348" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Los Angeles FC</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Los Angeles Galaxy</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>3</v>
+      </c>
+      <c r="E349" t="n">
+        <v>3</v>
+      </c>
+      <c r="F349" t="n">
+        <v>1326562</v>
+      </c>
+      <c r="G349" t="n">
+        <v>4</v>
+      </c>
+      <c r="H349" t="n">
+        <v>3</v>
+      </c>
+      <c r="I349" t="n">
+        <v>3</v>
+      </c>
+      <c r="J349" t="n">
+        <v>4</v>
+      </c>
+      <c r="K349" t="n">
+        <v>1</v>
+      </c>
+      <c r="L349" t="n">
+        <v>0</v>
+      </c>
+      <c r="M349" t="n">
+        <v>0</v>
+      </c>
+      <c r="N349" t="n">
+        <v>0</v>
+      </c>
+      <c r="O349" t="n">
+        <v>3</v>
+      </c>
+      <c r="P349" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q349" t="inlineStr">
+        <is>
+          <t>35%</t>
+        </is>
+      </c>
+      <c r="R349" t="inlineStr">
+        <is>
+          <t>65%</t>
+        </is>
+      </c>
+      <c r="S349" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Portland Timbers</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Minnesota United FC</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>1</v>
+      </c>
+      <c r="E350" t="n">
+        <v>1</v>
+      </c>
+      <c r="F350" t="n">
+        <v>1326563</v>
+      </c>
+      <c r="G350" t="n">
+        <v>6</v>
+      </c>
+      <c r="H350" t="n">
+        <v>3</v>
+      </c>
+      <c r="I350" t="n">
+        <v>1</v>
+      </c>
+      <c r="J350" t="n">
+        <v>3</v>
+      </c>
+      <c r="K350" t="n">
+        <v>0</v>
+      </c>
+      <c r="L350" t="n">
+        <v>0</v>
+      </c>
+      <c r="M350" t="n">
+        <v>0</v>
+      </c>
+      <c r="N350" t="n">
+        <v>0</v>
+      </c>
+      <c r="O350" t="n">
+        <v>1</v>
+      </c>
+      <c r="P350" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q350" t="inlineStr">
+        <is>
+          <t>64%</t>
+        </is>
+      </c>
+      <c r="R350" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
+      <c r="S350" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>2025-07-20</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>1</v>
+      </c>
+      <c r="E351" t="n">
+        <v>1</v>
+      </c>
+      <c r="F351" t="n">
+        <v>1326732</v>
+      </c>
+      <c r="G351" t="n">
+        <v>10</v>
+      </c>
+      <c r="H351" t="n">
+        <v>2</v>
+      </c>
+      <c r="I351" t="n">
+        <v>1</v>
+      </c>
+      <c r="J351" t="n">
+        <v>3</v>
+      </c>
+      <c r="K351" t="n">
+        <v>0</v>
+      </c>
+      <c r="L351" t="n">
+        <v>0</v>
+      </c>
+      <c r="M351" t="n">
+        <v>0</v>
+      </c>
+      <c r="N351" t="n">
+        <v>0</v>
+      </c>
+      <c r="O351" t="n">
+        <v>1</v>
+      </c>
+      <c r="P351" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q351" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="R351" t="inlineStr">
+        <is>
+          <t>38%</t>
+        </is>
+      </c>
+      <c r="S351" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregada liga de Dinamarca
</commit_message>
<xml_diff>
--- a/Ligas/Liga_MLS_2025.xlsx
+++ b/Ligas/Liga_MLS_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435FBC80-E0D7-4D6C-B533-A3303CFBBF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F68F8B-7533-4FFA-8FCE-F372F9BE5EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="125">
   <si>
     <t>Fecha</t>
   </si>
@@ -387,6 +387,15 @@
   <si>
     <t>2025-08-11</t>
   </si>
+  <si>
+    <t>2025-08-16</t>
+  </si>
+  <si>
+    <t>2025-08-17</t>
+  </si>
+  <si>
+    <t>2025-08-18</t>
+  </si>
 </sst>
 </file>
 
@@ -748,13 +757,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W379"/>
+  <dimension ref="A1:W394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="J379" sqref="J379"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="J391" sqref="J391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -23115,6 +23127,891 @@
       </c>
       <c r="S379" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="380" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>122</v>
+      </c>
+      <c r="B380" t="s">
+        <v>36</v>
+      </c>
+      <c r="C380" t="s">
+        <v>33</v>
+      </c>
+      <c r="D380">
+        <v>1</v>
+      </c>
+      <c r="E380">
+        <v>1</v>
+      </c>
+      <c r="F380">
+        <v>1326598</v>
+      </c>
+      <c r="G380">
+        <v>2</v>
+      </c>
+      <c r="H380">
+        <v>7</v>
+      </c>
+      <c r="I380">
+        <v>0</v>
+      </c>
+      <c r="J380">
+        <v>1</v>
+      </c>
+      <c r="K380">
+        <v>0</v>
+      </c>
+      <c r="L380">
+        <v>0</v>
+      </c>
+      <c r="M380">
+        <v>0</v>
+      </c>
+      <c r="N380">
+        <v>1</v>
+      </c>
+      <c r="O380">
+        <v>1</v>
+      </c>
+      <c r="P380">
+        <v>0</v>
+      </c>
+      <c r="Q380">
+        <v>44</v>
+      </c>
+      <c r="R380">
+        <v>56</v>
+      </c>
+      <c r="S380" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="381" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>122</v>
+      </c>
+      <c r="B381" t="s">
+        <v>39</v>
+      </c>
+      <c r="C381" t="s">
+        <v>29</v>
+      </c>
+      <c r="D381">
+        <v>1</v>
+      </c>
+      <c r="E381">
+        <v>0</v>
+      </c>
+      <c r="F381">
+        <v>1326596</v>
+      </c>
+      <c r="G381">
+        <v>1</v>
+      </c>
+      <c r="H381">
+        <v>2</v>
+      </c>
+      <c r="I381">
+        <v>2</v>
+      </c>
+      <c r="J381">
+        <v>0</v>
+      </c>
+      <c r="K381">
+        <v>0</v>
+      </c>
+      <c r="L381">
+        <v>0</v>
+      </c>
+      <c r="M381">
+        <v>0</v>
+      </c>
+      <c r="N381">
+        <v>0</v>
+      </c>
+      <c r="O381">
+        <v>1</v>
+      </c>
+      <c r="P381">
+        <v>0</v>
+      </c>
+      <c r="Q381">
+        <v>51</v>
+      </c>
+      <c r="R381">
+        <v>49</v>
+      </c>
+      <c r="S381" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="382" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>122</v>
+      </c>
+      <c r="B382" t="s">
+        <v>45</v>
+      </c>
+      <c r="C382" t="s">
+        <v>24</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382">
+        <v>2</v>
+      </c>
+      <c r="F382">
+        <v>1326595</v>
+      </c>
+      <c r="G382">
+        <v>4</v>
+      </c>
+      <c r="H382">
+        <v>3</v>
+      </c>
+      <c r="I382">
+        <v>1</v>
+      </c>
+      <c r="J382">
+        <v>1</v>
+      </c>
+      <c r="K382">
+        <v>0</v>
+      </c>
+      <c r="L382">
+        <v>0</v>
+      </c>
+      <c r="M382">
+        <v>0</v>
+      </c>
+      <c r="N382">
+        <v>0</v>
+      </c>
+      <c r="O382">
+        <v>0</v>
+      </c>
+      <c r="P382">
+        <v>2</v>
+      </c>
+      <c r="Q382">
+        <v>48</v>
+      </c>
+      <c r="R382">
+        <v>52</v>
+      </c>
+      <c r="S382" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="383" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>122</v>
+      </c>
+      <c r="B383" t="s">
+        <v>32</v>
+      </c>
+      <c r="C383" t="s">
+        <v>35</v>
+      </c>
+      <c r="D383">
+        <v>1</v>
+      </c>
+      <c r="E383">
+        <v>1</v>
+      </c>
+      <c r="F383">
+        <v>1326594</v>
+      </c>
+      <c r="G383">
+        <v>2</v>
+      </c>
+      <c r="H383">
+        <v>4</v>
+      </c>
+      <c r="I383">
+        <v>2</v>
+      </c>
+      <c r="J383">
+        <v>4</v>
+      </c>
+      <c r="K383">
+        <v>0</v>
+      </c>
+      <c r="L383">
+        <v>0</v>
+      </c>
+      <c r="M383">
+        <v>1</v>
+      </c>
+      <c r="N383">
+        <v>1</v>
+      </c>
+      <c r="O383">
+        <v>0</v>
+      </c>
+      <c r="P383">
+        <v>0</v>
+      </c>
+      <c r="Q383">
+        <v>58</v>
+      </c>
+      <c r="R383">
+        <v>42</v>
+      </c>
+      <c r="S383" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="384" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>122</v>
+      </c>
+      <c r="B384" t="s">
+        <v>40</v>
+      </c>
+      <c r="C384" t="s">
+        <v>57</v>
+      </c>
+      <c r="D384">
+        <v>3</v>
+      </c>
+      <c r="E384">
+        <v>1</v>
+      </c>
+      <c r="F384">
+        <v>1326593</v>
+      </c>
+      <c r="G384">
+        <v>13</v>
+      </c>
+      <c r="H384">
+        <v>2</v>
+      </c>
+      <c r="I384">
+        <v>0</v>
+      </c>
+      <c r="J384">
+        <v>0</v>
+      </c>
+      <c r="K384">
+        <v>0</v>
+      </c>
+      <c r="L384">
+        <v>0</v>
+      </c>
+      <c r="M384">
+        <v>1</v>
+      </c>
+      <c r="N384">
+        <v>0</v>
+      </c>
+      <c r="O384">
+        <v>2</v>
+      </c>
+      <c r="P384">
+        <v>1</v>
+      </c>
+      <c r="Q384">
+        <v>46</v>
+      </c>
+      <c r="R384">
+        <v>54</v>
+      </c>
+      <c r="S384" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="385" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>122</v>
+      </c>
+      <c r="B385" t="s">
+        <v>51</v>
+      </c>
+      <c r="C385" t="s">
+        <v>53</v>
+      </c>
+      <c r="D385">
+        <v>1</v>
+      </c>
+      <c r="E385">
+        <v>0</v>
+      </c>
+      <c r="F385">
+        <v>1326592</v>
+      </c>
+      <c r="G385">
+        <v>3</v>
+      </c>
+      <c r="H385">
+        <v>5</v>
+      </c>
+      <c r="I385">
+        <v>1</v>
+      </c>
+      <c r="J385">
+        <v>4</v>
+      </c>
+      <c r="K385">
+        <v>0</v>
+      </c>
+      <c r="L385">
+        <v>0</v>
+      </c>
+      <c r="M385">
+        <v>1</v>
+      </c>
+      <c r="N385">
+        <v>0</v>
+      </c>
+      <c r="O385">
+        <v>0</v>
+      </c>
+      <c r="P385">
+        <v>0</v>
+      </c>
+      <c r="Q385">
+        <v>51</v>
+      </c>
+      <c r="R385">
+        <v>49</v>
+      </c>
+      <c r="S385" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="386" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>123</v>
+      </c>
+      <c r="B386" t="s">
+        <v>25</v>
+      </c>
+      <c r="C386" t="s">
+        <v>50</v>
+      </c>
+      <c r="D386">
+        <v>1</v>
+      </c>
+      <c r="E386">
+        <v>0</v>
+      </c>
+      <c r="F386">
+        <v>1326601</v>
+      </c>
+      <c r="G386">
+        <v>3</v>
+      </c>
+      <c r="H386">
+        <v>8</v>
+      </c>
+      <c r="I386">
+        <v>2</v>
+      </c>
+      <c r="J386">
+        <v>1</v>
+      </c>
+      <c r="K386">
+        <v>0</v>
+      </c>
+      <c r="L386">
+        <v>0</v>
+      </c>
+      <c r="M386">
+        <v>0</v>
+      </c>
+      <c r="N386">
+        <v>0</v>
+      </c>
+      <c r="O386">
+        <v>1</v>
+      </c>
+      <c r="P386">
+        <v>0</v>
+      </c>
+      <c r="Q386">
+        <v>29</v>
+      </c>
+      <c r="R386">
+        <v>71</v>
+      </c>
+      <c r="S386" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="387" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>123</v>
+      </c>
+      <c r="B387" t="s">
+        <v>46</v>
+      </c>
+      <c r="C387" t="s">
+        <v>43</v>
+      </c>
+      <c r="D387">
+        <v>1</v>
+      </c>
+      <c r="E387">
+        <v>1</v>
+      </c>
+      <c r="F387">
+        <v>1326599</v>
+      </c>
+      <c r="G387">
+        <v>6</v>
+      </c>
+      <c r="H387">
+        <v>3</v>
+      </c>
+      <c r="I387">
+        <v>2</v>
+      </c>
+      <c r="J387">
+        <v>3</v>
+      </c>
+      <c r="K387">
+        <v>0</v>
+      </c>
+      <c r="L387">
+        <v>0</v>
+      </c>
+      <c r="M387">
+        <v>0</v>
+      </c>
+      <c r="N387">
+        <v>1</v>
+      </c>
+      <c r="O387">
+        <v>1</v>
+      </c>
+      <c r="P387">
+        <v>0</v>
+      </c>
+      <c r="Q387">
+        <v>65</v>
+      </c>
+      <c r="R387">
+        <v>35</v>
+      </c>
+      <c r="S387" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="388" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>123</v>
+      </c>
+      <c r="B388" t="s">
+        <v>49</v>
+      </c>
+      <c r="C388" t="s">
+        <v>31</v>
+      </c>
+      <c r="D388">
+        <v>3</v>
+      </c>
+      <c r="E388">
+        <v>1</v>
+      </c>
+      <c r="F388">
+        <v>1326602</v>
+      </c>
+      <c r="G388">
+        <v>3</v>
+      </c>
+      <c r="H388">
+        <v>4</v>
+      </c>
+      <c r="I388">
+        <v>2</v>
+      </c>
+      <c r="J388">
+        <v>0</v>
+      </c>
+      <c r="K388">
+        <v>0</v>
+      </c>
+      <c r="L388">
+        <v>0</v>
+      </c>
+      <c r="M388">
+        <v>1</v>
+      </c>
+      <c r="N388">
+        <v>1</v>
+      </c>
+      <c r="O388">
+        <v>2</v>
+      </c>
+      <c r="P388">
+        <v>0</v>
+      </c>
+      <c r="Q388">
+        <v>44</v>
+      </c>
+      <c r="R388">
+        <v>56</v>
+      </c>
+      <c r="S388" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="389" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>123</v>
+      </c>
+      <c r="B389" t="s">
+        <v>34</v>
+      </c>
+      <c r="C389" t="s">
+        <v>48</v>
+      </c>
+      <c r="D389">
+        <v>3</v>
+      </c>
+      <c r="E389">
+        <v>2</v>
+      </c>
+      <c r="F389">
+        <v>1326600</v>
+      </c>
+      <c r="G389">
+        <v>6</v>
+      </c>
+      <c r="H389">
+        <v>2</v>
+      </c>
+      <c r="I389">
+        <v>0</v>
+      </c>
+      <c r="J389">
+        <v>4</v>
+      </c>
+      <c r="K389">
+        <v>0</v>
+      </c>
+      <c r="L389">
+        <v>0</v>
+      </c>
+      <c r="M389">
+        <v>1</v>
+      </c>
+      <c r="N389">
+        <v>0</v>
+      </c>
+      <c r="O389">
+        <v>2</v>
+      </c>
+      <c r="P389">
+        <v>2</v>
+      </c>
+      <c r="Q389">
+        <v>51</v>
+      </c>
+      <c r="R389">
+        <v>49</v>
+      </c>
+      <c r="S389" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="390" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>123</v>
+      </c>
+      <c r="B390" t="s">
+        <v>54</v>
+      </c>
+      <c r="C390" t="s">
+        <v>38</v>
+      </c>
+      <c r="D390">
+        <v>2</v>
+      </c>
+      <c r="E390">
+        <v>3</v>
+      </c>
+      <c r="F390">
+        <v>1326603</v>
+      </c>
+      <c r="G390">
+        <v>6</v>
+      </c>
+      <c r="H390">
+        <v>3</v>
+      </c>
+      <c r="I390">
+        <v>2</v>
+      </c>
+      <c r="J390">
+        <v>1</v>
+      </c>
+      <c r="K390">
+        <v>0</v>
+      </c>
+      <c r="L390">
+        <v>0</v>
+      </c>
+      <c r="M390">
+        <v>1</v>
+      </c>
+      <c r="N390">
+        <v>3</v>
+      </c>
+      <c r="O390">
+        <v>1</v>
+      </c>
+      <c r="P390">
+        <v>0</v>
+      </c>
+      <c r="Q390">
+        <v>58</v>
+      </c>
+      <c r="R390">
+        <v>42</v>
+      </c>
+      <c r="S390" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="391" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>123</v>
+      </c>
+      <c r="B391" t="s">
+        <v>28</v>
+      </c>
+      <c r="C391" t="s">
+        <v>47</v>
+      </c>
+      <c r="D391">
+        <v>3</v>
+      </c>
+      <c r="E391">
+        <v>1</v>
+      </c>
+      <c r="F391">
+        <v>1326597</v>
+      </c>
+      <c r="G391">
+        <v>6</v>
+      </c>
+      <c r="H391">
+        <v>4</v>
+      </c>
+      <c r="I391">
+        <v>0</v>
+      </c>
+      <c r="J391">
+        <v>0</v>
+      </c>
+      <c r="K391">
+        <v>0</v>
+      </c>
+      <c r="L391">
+        <v>0</v>
+      </c>
+      <c r="M391">
+        <v>1</v>
+      </c>
+      <c r="N391">
+        <v>1</v>
+      </c>
+      <c r="O391">
+        <v>2</v>
+      </c>
+      <c r="P391">
+        <v>0</v>
+      </c>
+      <c r="Q391">
+        <v>54</v>
+      </c>
+      <c r="R391">
+        <v>46</v>
+      </c>
+      <c r="S391" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="392" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>123</v>
+      </c>
+      <c r="B392" t="s">
+        <v>41</v>
+      </c>
+      <c r="C392" t="s">
+        <v>44</v>
+      </c>
+      <c r="D392">
+        <v>2</v>
+      </c>
+      <c r="E392">
+        <v>1</v>
+      </c>
+      <c r="F392">
+        <v>1326604</v>
+      </c>
+      <c r="G392">
+        <v>2</v>
+      </c>
+      <c r="H392">
+        <v>3</v>
+      </c>
+      <c r="I392">
+        <v>3</v>
+      </c>
+      <c r="J392">
+        <v>2</v>
+      </c>
+      <c r="K392">
+        <v>0</v>
+      </c>
+      <c r="L392">
+        <v>0</v>
+      </c>
+      <c r="M392">
+        <v>1</v>
+      </c>
+      <c r="N392">
+        <v>1</v>
+      </c>
+      <c r="O392">
+        <v>1</v>
+      </c>
+      <c r="P392">
+        <v>0</v>
+      </c>
+      <c r="Q392">
+        <v>54</v>
+      </c>
+      <c r="R392">
+        <v>46</v>
+      </c>
+      <c r="S392" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="393" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>123</v>
+      </c>
+      <c r="B393" t="s">
+        <v>52</v>
+      </c>
+      <c r="C393" t="s">
+        <v>58</v>
+      </c>
+      <c r="D393">
+        <v>1</v>
+      </c>
+      <c r="E393">
+        <v>2</v>
+      </c>
+      <c r="F393">
+        <v>1326735</v>
+      </c>
+      <c r="G393">
+        <v>3</v>
+      </c>
+      <c r="H393">
+        <v>6</v>
+      </c>
+      <c r="I393">
+        <v>2</v>
+      </c>
+      <c r="J393">
+        <v>3</v>
+      </c>
+      <c r="K393">
+        <v>0</v>
+      </c>
+      <c r="L393">
+        <v>0</v>
+      </c>
+      <c r="M393">
+        <v>0</v>
+      </c>
+      <c r="N393">
+        <v>0</v>
+      </c>
+      <c r="O393">
+        <v>1</v>
+      </c>
+      <c r="P393">
+        <v>2</v>
+      </c>
+      <c r="Q393">
+        <v>44</v>
+      </c>
+      <c r="R393">
+        <v>56</v>
+      </c>
+      <c r="S393" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="394" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>124</v>
+      </c>
+      <c r="B394" t="s">
+        <v>55</v>
+      </c>
+      <c r="C394" t="s">
+        <v>42</v>
+      </c>
+      <c r="D394">
+        <v>1</v>
+      </c>
+      <c r="E394">
+        <v>1</v>
+      </c>
+      <c r="F394">
+        <v>1326605</v>
+      </c>
+      <c r="G394">
+        <v>5</v>
+      </c>
+      <c r="H394">
+        <v>4</v>
+      </c>
+      <c r="I394">
+        <v>2</v>
+      </c>
+      <c r="J394">
+        <v>5</v>
+      </c>
+      <c r="K394">
+        <v>0</v>
+      </c>
+      <c r="L394">
+        <v>1</v>
+      </c>
+      <c r="M394">
+        <v>1</v>
+      </c>
+      <c r="N394">
+        <v>0</v>
+      </c>
+      <c r="O394">
+        <v>0</v>
+      </c>
+      <c r="P394">
+        <v>1</v>
+      </c>
+      <c r="Q394">
+        <v>53</v>
+      </c>
+      <c r="R394">
+        <v>47</v>
+      </c>
+      <c r="S394" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>